<commit_message>
Added additional site for testing
</commit_message>
<xml_diff>
--- a/web-scraping/sites/generic_one_table/pages.xlsx
+++ b/web-scraping/sites/generic_one_table/pages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>url</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>class2</t>
+  </si>
+  <si>
+    <t>vgchartz_2</t>
   </si>
 </sst>
 </file>
@@ -506,13 +509,27 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="5"/>

</xml_diff>

<commit_message>
Removed one row from file
</commit_message>
<xml_diff>
--- a/web-scraping/sites/generic_one_table/pages.xlsx
+++ b/web-scraping/sites/generic_one_table/pages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>url</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>class2</t>
-  </si>
-  <si>
-    <t>vgchartz_2</t>
   </si>
 </sst>
 </file>
@@ -447,7 +444,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -509,31 +506,17 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -549,15 +532,6 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>